<commit_message>
Re-write the Login page Complete data validation Other minor updates
</commit_message>
<xml_diff>
--- a/SalesExpense/static/media/客户档案模板.xlsx
+++ b/SalesExpense/static/media/客户档案模板.xlsx
@@ -198,7 +198,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="0" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="20">
@@ -402,182 +402,182 @@
     </border>
   </borders>
   <cellStyleXfs count="62">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyBorder="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyBorder="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyBorder="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+  <cellXfs count="32">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="10" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -585,18 +585,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="10" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -605,13 +605,13 @@
     <xf numFmtId="9" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="177" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -620,38 +620,38 @@
     <xf numFmtId="9" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="177" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="10" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="10" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -666,6 +666,9 @@
     <xf numFmtId="177" fontId="10" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1049,7 +1052,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1169,7 +1172,7 @@
       <c r="M2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="22">
+      <c r="N2" s="30">
         <v>13366839490</v>
       </c>
       <c r="O2" s="9">
@@ -1181,7 +1184,7 @@
       <c r="Q2" s="9">
         <v>390</v>
       </c>
-      <c r="R2" s="30">
+      <c r="R2" s="31">
         <v>54</v>
       </c>
       <c r="S2" s="9">

</xml_diff>

<commit_message>
Reconstruc Model by requirement Add Treemap view of analysis module
</commit_message>
<xml_diff>
--- a/SalesExpense/static/media/客户档案模板.xlsx
+++ b/SalesExpense/static/media/客户档案模板.xlsx
@@ -10,7 +10,7 @@
     <sheet name="客户档案" sheetId="6" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">客户档案!$A$1:$S$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">客户档案!$A$1:$R$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -292,7 +292,9 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-必须是0或正整数</t>
+必须是0-100之间的整数
+本列请特别注意不要填小数或百分比
+（如想表达相关病人比例为40%，请填40）</t>
         </r>
       </text>
     </comment>
@@ -318,39 +320,11 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-必须是0-100之间的整数
-本列请特别注意不要填小数或百分比
-（如想表达相关病人比例为40%，请填40）</t>
+必须为0或正整数</t>
         </r>
       </text>
     </comment>
     <comment ref="S1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-必须为0或正整数</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -381,7 +355,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>李鲜</t>
   </si>
@@ -400,10 +374,6 @@
   <si>
     <t>每半天
 门诊量</t>
-  </si>
-  <si>
-    <t>月累计
-门诊病人数</t>
   </si>
   <si>
     <t>相关病人
@@ -1344,11 +1314,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1360,26 +1330,26 @@
     <col min="8" max="12" width="8.625" style="10" customWidth="1"/>
     <col min="13" max="13" width="12.625" style="10" customWidth="1"/>
     <col min="14" max="14" width="11.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="8.625" style="11" customWidth="1"/>
-    <col min="18" max="18" width="8.625" style="13" customWidth="1"/>
-    <col min="19" max="20" width="8.625" style="11" customWidth="1"/>
-    <col min="21" max="21" width="9" style="5"/>
-    <col min="22" max="22" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9" style="5"/>
+    <col min="15" max="16" width="8.625" style="11" customWidth="1"/>
+    <col min="17" max="17" width="8.625" style="13" customWidth="1"/>
+    <col min="18" max="19" width="8.625" style="11" customWidth="1"/>
+    <col min="20" max="20" width="9" style="5"/>
+    <col min="21" max="21" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="57">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="57">
       <c r="A1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>11</v>
-      </c>
       <c r="C1" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -1388,54 +1358,51 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" s="17" t="s">
-        <v>22</v>
+      <c r="R1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:19">
       <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
@@ -1444,31 +1411,31 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N2" s="19">
         <v>13366839490</v>
@@ -1479,25 +1446,22 @@
       <c r="P2" s="8">
         <v>30</v>
       </c>
-      <c r="Q2" s="8">
-        <v>390</v>
-      </c>
-      <c r="R2" s="21">
+      <c r="Q2" s="21">
         <v>54</v>
       </c>
-      <c r="S2" s="8">
+      <c r="R2" s="8">
         <v>231</v>
       </c>
-      <c r="T2" s="22" t="s">
-        <v>33</v>
+      <c r="S2" s="22" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S2"/>
+  <autoFilter ref="A1:R2"/>
   <dataConsolidate/>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:S2 O2:Q2">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:R2 O2:P2">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Modified hp level choice set Removed distintct validation on Name field
</commit_message>
<xml_diff>
--- a/SalesExpense/static/media/客户档案模板.xlsx
+++ b/SalesExpense/static/media/客户档案模板.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC051BA-3DDD-4098-A671-FC3E2D4655A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="884"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="客户档案" sheetId="6" r:id="rId1"/>
@@ -13,24 +14,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">客户档案!$A$1:$R$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -85,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -112,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -134,11 +127,11 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-本列只接受A、B、C、D四个选项</t>
+本列只接受A、B、C、D、旗舰社区、普通社区6个选项</t>
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -166,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -192,7 +185,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{0BA1B8C5-ED85-40F3-B6B3-21C2FD72862F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+本列只接受院长、副院长、主任医师、副主任医师、主治医师、住院医师、其他7各选项</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -218,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -244,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -270,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -298,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -324,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -489,12 +506,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,6 +652,19 @@
       <color theme="1"/>
       <name val="微软雅黑"/>
       <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -942,67 +972,67 @@
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
-    <cellStyle name="百分比 10" xfId="35"/>
-    <cellStyle name="百分比 10 2" xfId="51"/>
-    <cellStyle name="百分比 2" xfId="3"/>
-    <cellStyle name="百分比 3 4" xfId="41"/>
-    <cellStyle name="百分比 4" xfId="23"/>
+    <cellStyle name="百分比 10" xfId="35" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="百分比 10 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="百分比 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="百分比 3 4" xfId="41" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="百分比 4" xfId="23" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="20"/>
-    <cellStyle name="常规 11" xfId="25"/>
-    <cellStyle name="常规 11 2" xfId="17"/>
-    <cellStyle name="常规 11 2 2" xfId="52"/>
-    <cellStyle name="常规 11 3" xfId="24"/>
-    <cellStyle name="常规 12" xfId="38"/>
-    <cellStyle name="常规 12 18 2 2" xfId="16"/>
-    <cellStyle name="常规 12 18 2 2 2" xfId="21"/>
-    <cellStyle name="常规 12 18 2 2 4" xfId="42"/>
-    <cellStyle name="常规 12 18 3" xfId="19"/>
-    <cellStyle name="常规 12 19" xfId="36"/>
-    <cellStyle name="常规 12 19 2" xfId="47"/>
-    <cellStyle name="常规 12 2" xfId="44"/>
-    <cellStyle name="常规 13" xfId="43"/>
-    <cellStyle name="常规 14" xfId="33"/>
-    <cellStyle name="常规 16" xfId="37"/>
-    <cellStyle name="常规 17" xfId="12"/>
-    <cellStyle name="常规 19" xfId="30"/>
-    <cellStyle name="常规 2" xfId="2"/>
-    <cellStyle name="常规 2 10" xfId="10"/>
-    <cellStyle name="常规 2 10 15" xfId="15"/>
-    <cellStyle name="常规 2 10 15 2" xfId="49"/>
-    <cellStyle name="常规 2 10 2" xfId="29"/>
-    <cellStyle name="常规 2 2" xfId="9"/>
-    <cellStyle name="常规 2 25" xfId="34"/>
-    <cellStyle name="常规 2 26 2" xfId="13"/>
-    <cellStyle name="常规 2 26 2 2" xfId="18"/>
-    <cellStyle name="常规 2 3" xfId="8"/>
-    <cellStyle name="常规 2 3 2" xfId="11"/>
-    <cellStyle name="常规 2 3 2 2" xfId="57"/>
-    <cellStyle name="常规 2 3 3" xfId="14"/>
-    <cellStyle name="常规 2 3 3 3" xfId="26"/>
-    <cellStyle name="常规 2 3 5" xfId="31"/>
-    <cellStyle name="常规 2 3 6" xfId="32"/>
-    <cellStyle name="常规 2 5" xfId="58"/>
-    <cellStyle name="常规 2 6" xfId="27"/>
-    <cellStyle name="常规 2 6 2" xfId="5"/>
-    <cellStyle name="常规 2 6 2 2" xfId="28"/>
-    <cellStyle name="常规 2 6 2 2 2" xfId="50"/>
-    <cellStyle name="常规 2 6 2 3" xfId="39"/>
-    <cellStyle name="常规 2 6 2 4" xfId="54"/>
-    <cellStyle name="常规 2 6 2 5" xfId="56"/>
-    <cellStyle name="常规 2 6 3 9 2" xfId="46"/>
-    <cellStyle name="常规 2 6 4 3" xfId="55"/>
-    <cellStyle name="常规 23" xfId="61"/>
-    <cellStyle name="常规 3" xfId="7"/>
-    <cellStyle name="常规 3 2" xfId="22"/>
-    <cellStyle name="常规 3 3" xfId="45"/>
-    <cellStyle name="常规 3 4" xfId="53"/>
-    <cellStyle name="常规 3 5 2" xfId="48"/>
-    <cellStyle name="常规 3 6" xfId="40"/>
-    <cellStyle name="常规 4" xfId="6"/>
-    <cellStyle name="常规 5" xfId="60"/>
-    <cellStyle name="常规 7" xfId="59"/>
-    <cellStyle name="常规_Sheet1_1" xfId="4"/>
+    <cellStyle name="常规 10" xfId="20" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="常规 11" xfId="25" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="常规 11 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="常规 11 2 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="常规 11 3" xfId="24" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="常规 12" xfId="38" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="常规 12 18 2 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="常规 12 18 2 2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="常规 12 18 2 2 4" xfId="42" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="常规 12 18 3" xfId="19" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="常规 12 19" xfId="36" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="常规 12 19 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="常规 12 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="常规 13" xfId="43" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="常规 14" xfId="33" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="常规 16" xfId="37" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="常规 17" xfId="12" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="常规 19" xfId="30" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="常规 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="常规 2 10" xfId="10" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="常规 2 10 15" xfId="15" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="常规 2 10 15 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="常规 2 10 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="常规 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="常规 2 25" xfId="34" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="常规 2 26 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="常规 2 26 2 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="常规 2 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="常规 2 3 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="常规 2 3 2 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="常规 2 3 3" xfId="14" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="常规 2 3 3 3" xfId="26" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="常规 2 3 5" xfId="31" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="常规 2 3 6" xfId="32" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="常规 2 5" xfId="58" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="常规 2 6" xfId="27" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="常规 2 6 2" xfId="5" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="常规 2 6 2 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="常规 2 6 2 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="常规 2 6 2 3" xfId="39" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="常规 2 6 2 4" xfId="54" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="常规 2 6 2 5" xfId="56" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="常规 2 6 3 9 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="常规 2 6 4 3" xfId="55" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="常规 23" xfId="61" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="常规 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="常规 3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="常规 3 3" xfId="45" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="常规 3 4" xfId="53" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="常规 3 5 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="常规 3 6" xfId="40" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="常规 4" xfId="6" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="常规 5" xfId="60" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="常规 7" xfId="59" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="常规_Sheet1_1" xfId="4" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1012,7 +1042,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
-    <tableStyle name="表样式 1" pivot="0" count="1">
+    <tableStyle name="表样式 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="0"/>
     </tableStyle>
   </tableStyles>
@@ -1028,7 +1058,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1103,6 +1133,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1138,6 +1185,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1313,32 +1377,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O7" sqref="O7"/>
+      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="8.625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="12.625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="27.375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="10.375" style="12" customWidth="1"/>
-    <col min="8" max="12" width="8.625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="12.625" style="10" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.625" style="11" customWidth="1"/>
-    <col min="17" max="17" width="8.625" style="13" customWidth="1"/>
-    <col min="18" max="19" width="8.625" style="11" customWidth="1"/>
+    <col min="1" max="4" width="8.6328125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="27.36328125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" style="12" customWidth="1"/>
+    <col min="8" max="12" width="8.6328125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="11.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="8.6328125" style="11" customWidth="1"/>
+    <col min="17" max="17" width="8.6328125" style="13" customWidth="1"/>
+    <col min="18" max="19" width="8.6328125" style="11" customWidth="1"/>
     <col min="20" max="20" width="9" style="5"/>
     <col min="21" max="21" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="57">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="67.5" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
@@ -1397,7 +1461,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>19</v>
       </c>
@@ -1457,11 +1521,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R2"/>
+  <autoFilter ref="A1:R2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataConsolidate/>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:R2 O2:P2">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:R2 O2:P2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add the support toward different BUs
</commit_message>
<xml_diff>
--- a/SalesExpense/static/media/客户档案模板.xlsx
+++ b/SalesExpense/static/media/客户档案模板.xlsx
@@ -1,29 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC051BA-3DDD-4098-A671-FC3E2D4655A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="884" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="38625" windowHeight="21225" tabRatio="884"/>
   </bookViews>
   <sheets>
     <sheet name="客户档案" sheetId="6" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">客户档案!$A$1:$R$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">客户档案!$B$1:$S$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+请使用地理方位而不是RD名字</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -105,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -131,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{0BA1B8C5-ED85-40F3-B6B3-21C2FD72862F}">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -193,6 +218,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>作者:</t>
@@ -202,6 +228,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
@@ -209,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -231,11 +258,11 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-本列可以为空</t>
+本列可以为空；即使填写为了保护隐私也不会上传至系统，可在本地excel保留</t>
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -261,7 +288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -287,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -315,7 +342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -341,7 +368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -372,7 +399,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>李鲜</t>
   </si>
@@ -447,10 +474,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>周雪莲</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>王钢</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -500,18 +523,30 @@
   </si>
   <si>
     <t>本行为示例，上传前请删除</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>团队</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>血压团队</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>华北区</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -654,21 +689,8 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -696,6 +718,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -953,10 +981,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -968,71 +992,75 @@
     </xf>
     <xf numFmtId="177" fontId="19" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
-    <cellStyle name="百分比 10" xfId="35" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="百分比 10 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="百分比 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="百分比 3 4" xfId="41" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="百分比 4" xfId="23" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="百分比 10" xfId="35"/>
+    <cellStyle name="百分比 10 2" xfId="51"/>
+    <cellStyle name="百分比 2" xfId="3"/>
+    <cellStyle name="百分比 3 4" xfId="41"/>
+    <cellStyle name="百分比 4" xfId="23"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="20" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="常规 11" xfId="25" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="常规 11 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="常规 11 2 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="常规 11 3" xfId="24" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="常规 12" xfId="38" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="常规 12 18 2 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="常规 12 18 2 2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="常规 12 18 2 2 4" xfId="42" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="常规 12 18 3" xfId="19" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="常规 12 19" xfId="36" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="常规 12 19 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="常规 12 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="常规 13" xfId="43" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="常规 14" xfId="33" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="常规 16" xfId="37" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="常规 17" xfId="12" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="常规 19" xfId="30" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="常规 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="常规 2 10" xfId="10" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="常规 2 10 15" xfId="15" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="常规 2 10 15 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="常规 2 10 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="常规 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="常规 2 25" xfId="34" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="常规 2 26 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="常规 2 26 2 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="常规 2 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="常规 2 3 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="常规 2 3 2 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="常规 2 3 3" xfId="14" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="常规 2 3 3 3" xfId="26" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="常规 2 3 5" xfId="31" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="常规 2 3 6" xfId="32" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="常规 2 5" xfId="58" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="常规 2 6" xfId="27" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="常规 2 6 2" xfId="5" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="常规 2 6 2 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="常规 2 6 2 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="常规 2 6 2 3" xfId="39" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="常规 2 6 2 4" xfId="54" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="常规 2 6 2 5" xfId="56" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="常规 2 6 3 9 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="常规 2 6 4 3" xfId="55" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="常规 23" xfId="61" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="常规 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="常规 3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="常规 3 3" xfId="45" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="常规 3 4" xfId="53" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="常规 3 5 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="常规 3 6" xfId="40" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="常规 4" xfId="6" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="常规 5" xfId="60" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="常规 7" xfId="59" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="常规_Sheet1_1" xfId="4" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="常规 10" xfId="20"/>
+    <cellStyle name="常规 11" xfId="25"/>
+    <cellStyle name="常规 11 2" xfId="17"/>
+    <cellStyle name="常规 11 2 2" xfId="52"/>
+    <cellStyle name="常规 11 3" xfId="24"/>
+    <cellStyle name="常规 12" xfId="38"/>
+    <cellStyle name="常规 12 18 2 2" xfId="16"/>
+    <cellStyle name="常规 12 18 2 2 2" xfId="21"/>
+    <cellStyle name="常规 12 18 2 2 4" xfId="42"/>
+    <cellStyle name="常规 12 18 3" xfId="19"/>
+    <cellStyle name="常规 12 19" xfId="36"/>
+    <cellStyle name="常规 12 19 2" xfId="47"/>
+    <cellStyle name="常规 12 2" xfId="44"/>
+    <cellStyle name="常规 13" xfId="43"/>
+    <cellStyle name="常规 14" xfId="33"/>
+    <cellStyle name="常规 16" xfId="37"/>
+    <cellStyle name="常规 17" xfId="12"/>
+    <cellStyle name="常规 19" xfId="30"/>
+    <cellStyle name="常规 2" xfId="2"/>
+    <cellStyle name="常规 2 10" xfId="10"/>
+    <cellStyle name="常规 2 10 15" xfId="15"/>
+    <cellStyle name="常规 2 10 15 2" xfId="49"/>
+    <cellStyle name="常规 2 10 2" xfId="29"/>
+    <cellStyle name="常规 2 2" xfId="9"/>
+    <cellStyle name="常规 2 25" xfId="34"/>
+    <cellStyle name="常规 2 26 2" xfId="13"/>
+    <cellStyle name="常规 2 26 2 2" xfId="18"/>
+    <cellStyle name="常规 2 3" xfId="8"/>
+    <cellStyle name="常规 2 3 2" xfId="11"/>
+    <cellStyle name="常规 2 3 2 2" xfId="57"/>
+    <cellStyle name="常规 2 3 3" xfId="14"/>
+    <cellStyle name="常规 2 3 3 3" xfId="26"/>
+    <cellStyle name="常规 2 3 5" xfId="31"/>
+    <cellStyle name="常规 2 3 6" xfId="32"/>
+    <cellStyle name="常规 2 5" xfId="58"/>
+    <cellStyle name="常规 2 6" xfId="27"/>
+    <cellStyle name="常规 2 6 2" xfId="5"/>
+    <cellStyle name="常规 2 6 2 2" xfId="28"/>
+    <cellStyle name="常规 2 6 2 2 2" xfId="50"/>
+    <cellStyle name="常规 2 6 2 3" xfId="39"/>
+    <cellStyle name="常规 2 6 2 4" xfId="54"/>
+    <cellStyle name="常规 2 6 2 5" xfId="56"/>
+    <cellStyle name="常规 2 6 3 9 2" xfId="46"/>
+    <cellStyle name="常规 2 6 4 3" xfId="55"/>
+    <cellStyle name="常规 23" xfId="61"/>
+    <cellStyle name="常规 3" xfId="7"/>
+    <cellStyle name="常规 3 2" xfId="22"/>
+    <cellStyle name="常规 3 3" xfId="45"/>
+    <cellStyle name="常规 3 4" xfId="53"/>
+    <cellStyle name="常规 3 5 2" xfId="48"/>
+    <cellStyle name="常规 3 6" xfId="40"/>
+    <cellStyle name="常规 4" xfId="6"/>
+    <cellStyle name="常规 5" xfId="60"/>
+    <cellStyle name="常规 7" xfId="59"/>
+    <cellStyle name="常规_Sheet1_1" xfId="4"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1042,7 +1070,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
-    <tableStyle name="表样式 1" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="表样式 1" pivot="0" count="1">
       <tableStyleElement type="wholeTable" dxfId="0"/>
     </tableStyle>
   </tableStyles>
@@ -1058,7 +1086,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1133,23 +1161,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1185,23 +1196,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1377,155 +1371,161 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="4" width="8.6328125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="27.36328125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="10.36328125" style="12" customWidth="1"/>
-    <col min="8" max="12" width="8.6328125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="12.6328125" style="10" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.6328125" style="11" customWidth="1"/>
-    <col min="17" max="17" width="8.6328125" style="13" customWidth="1"/>
-    <col min="18" max="19" width="8.6328125" style="11" customWidth="1"/>
-    <col min="20" max="20" width="9" style="5"/>
-    <col min="21" max="21" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9" style="5"/>
+    <col min="1" max="5" width="8.625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27.375" style="12" customWidth="1"/>
+    <col min="8" max="8" width="10.375" style="12" customWidth="1"/>
+    <col min="9" max="13" width="8.625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="12.625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="11.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.625" style="11" customWidth="1"/>
+    <col min="18" max="18" width="8.625" style="13" customWidth="1"/>
+    <col min="19" max="20" width="8.625" style="11" customWidth="1"/>
+    <col min="21" max="21" width="9" style="5"/>
+    <col min="22" max="22" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="67.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="57">
       <c r="A1" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="J2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="18">
+        <v>13366839490</v>
+      </c>
+      <c r="P2" s="8">
         <v>13</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="Q2" s="8">
         <v>30</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="R2" s="20">
+        <v>54</v>
+      </c>
+      <c r="S2" s="8">
+        <v>231</v>
+      </c>
+      <c r="T2" s="21" t="s">
         <v>31</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="19">
-        <v>13366839490</v>
-      </c>
-      <c r="O2" s="8">
-        <v>13</v>
-      </c>
-      <c r="P2" s="8">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="21">
-        <v>54</v>
-      </c>
-      <c r="R2" s="8">
-        <v>231</v>
-      </c>
-      <c r="S2" s="22" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:S2"/>
   <dataConsolidate/>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:R2 O2:P2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:S2 P2:Q2">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
continue construction of Reporting module
</commit_message>
<xml_diff>
--- a/SalesExpense/static/media/客户档案模板.xlsx
+++ b/SalesExpense/static/media/客户档案模板.xlsx
@@ -401,9 +401,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
-    <t>李鲜</t>
-  </si>
-  <si>
     <t>耿伟静</t>
   </si>
   <si>
@@ -526,15 +523,19 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>团队</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>血压团队</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>华北区</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>北中国</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>南北中国</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试1</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1376,7 +1377,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1398,108 +1399,108 @@
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" ht="57">
       <c r="A1" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="R1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="T1" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="F2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="M2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O2" s="18">
         <v>13366839490</v>
@@ -1517,7 +1518,7 @@
         <v>231</v>
       </c>
       <c r="T2" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for new structure of hp levels, depts and regions
</commit_message>
<xml_diff>
--- a/SalesExpense/static/media/客户档案模板.xlsx
+++ b/SalesExpense/static/media/客户档案模板.xlsx
@@ -44,7 +44,22 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-请使用地理方位而不是RD名字</t>
+请使用地理方位而不是RD名字
+北中国次列只接受“北一区”，“北二区”，“中区”3个选项；南中国只接受“南区”，“东区”2个选项</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>必须与用户名相同</t>
         </r>
       </text>
     </comment>
@@ -152,7 +167,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-本列只接受A、B、C、D、旗舰社区、普通社区6个选项</t>
+本列只接受D10-D1、旗舰社区、普通社区12个选项</t>
         </r>
       </text>
     </comment>
@@ -206,7 +221,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-本列只接受（心内科、神内科、老干科、肾内科、内分泌科、其他科室）6个选项</t>
+本列只接受（心内科、神内科、老干科、普内科、肾内科、内分泌科、其他科室、社区-全科、社区-其他）9个选项</t>
         </r>
       </text>
     </comment>
@@ -399,10 +414,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t>耿伟静</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>职称</t>
   </si>
@@ -459,10 +471,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>B</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>已开户</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -471,71 +479,81 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
+    <t>备注</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>心内科</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否双call</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>所在科室</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>地区经理</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>省/自治区/直辖市</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>H070000642</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国医学科学院阜外心血管病医院</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>朱兆仪</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>本行为示例，上传前请删除</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>北中国</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>南北中国</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>王钢</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>备注</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>心内科</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否双call</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>否</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>所在科室</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>地区经理</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>省/自治区/直辖市</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>北京</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>H070000642</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>中国医学科学院阜外心血管病医院</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>朱兆仪</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>本行为示例，上传前请删除</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>华北区</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>北中国</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>南北中国</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试1</t>
+  </si>
+  <si>
+    <t>TBA-北京1-05-06</t>
+  </si>
+  <si>
+    <t>测试2</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>D10</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>北一区</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>右侧列可无限扩展，和联系电话一样不会被上传至系统，方便DSM自己本地操作</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -926,7 +944,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="10" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -997,6 +1015,9 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -1373,11 +1394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1391,116 +1412,120 @@
     <col min="15" max="15" width="11.5" style="19" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="8.625" style="11" customWidth="1"/>
     <col min="18" max="18" width="8.625" style="13" customWidth="1"/>
-    <col min="19" max="20" width="8.625" style="11" customWidth="1"/>
+    <col min="19" max="19" width="8.625" style="11" customWidth="1"/>
+    <col min="20" max="20" width="18.5" style="11" customWidth="1"/>
     <col min="21" max="21" width="9" style="5"/>
     <col min="22" max="22" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="57">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="99.75">
       <c r="A1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="K2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="22" t="s">
+      <c r="N2" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T1" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>7</v>
       </c>
       <c r="O2" s="18">
         <v>13366839490</v>
@@ -1518,7 +1543,7 @@
         <v>231</v>
       </c>
       <c r="T2" s="21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1526,7 +1551,7 @@
   <dataConsolidate/>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:S2 P2:Q2">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:S2">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>